<commit_message>
PRIM updates to handle parent relationship to the Patient resource.
</commit_message>
<xml_diff>
--- a/PRIM/PRIM Public Comments.xlsx
+++ b/PRIM/PRIM Public Comments.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\IT-Infrastructure\PRIM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C17F32A-78C3-4634-90E3-DB2A71C4AA52}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25D62330-108C-46E0-92D9-F32FD322D2A4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="32477" windowHeight="16012" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="650" uniqueCount="318">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="657" uniqueCount="321">
   <si>
     <t>*Add RESTful Query to ATNA-comments due 2019-06-23</t>
   </si>
@@ -1261,6 +1261,15 @@
   <si>
     <t>I know I said above that I would not comment on the link/merge issue, but these sentence sound so much like an attempt to dance around the issue that they cannot be buried in a use case.   If the decisions is to go with "Link", then in the concepts section (X.4.1 currently blank) address this issue (link vs merge) head-on.</t>
   </si>
+  <si>
+    <t>3.Y1.4.1.2.1</t>
+  </si>
+  <si>
+    <t>how to handle patient parents in FHIR is vague so this needs to be clarified here.</t>
+  </si>
+  <si>
+    <t>Added text to use patient.link.other referenced a RelatedPerson with the link.type of seealso.</t>
+  </si>
 </sst>
 </file>
 
@@ -1344,7 +1353,7 @@
       <name val="Times New Roman"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1355,6 +1364,18 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFD9EAD3"/>
         <bgColor rgb="FFD9EAD3"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor rgb="FFD9EAD3"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -1439,7 +1460,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1554,6 +1575,23 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1883,8 +1921,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="F72" sqref="F72"/>
+    <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
+      <selection activeCell="F80" sqref="F80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="15" customHeight="1"/>
@@ -5336,12 +5374,35 @@
       <c r="W81" s="15"/>
       <c r="X81" s="15"/>
     </row>
-    <row r="82" spans="1:24" ht="15.75" customHeight="1">
-      <c r="D82" s="1"/>
-      <c r="E82" s="2"/>
-      <c r="F82" s="1"/>
-      <c r="G82" s="1"/>
-      <c r="I82" s="3"/>
+    <row r="82" spans="1:24" s="52" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A82" s="46" t="s">
+        <v>232</v>
+      </c>
+      <c r="B82" s="47" t="s">
+        <v>38</v>
+      </c>
+      <c r="C82" s="46">
+        <v>2</v>
+      </c>
+      <c r="D82" s="48" t="s">
+        <v>318</v>
+      </c>
+      <c r="E82" s="49">
+        <v>480</v>
+      </c>
+      <c r="F82" s="48" t="s">
+        <v>319</v>
+      </c>
+      <c r="G82" s="48"/>
+      <c r="H82" s="46" t="s">
+        <v>9</v>
+      </c>
+      <c r="I82" s="50" t="s">
+        <v>320</v>
+      </c>
+      <c r="J82" s="51" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="83" spans="1:24" ht="15.75" customHeight="1">
       <c r="D83" s="1"/>
@@ -11794,7 +11855,7 @@
           <x14:formula1>
             <xm:f>'Supplement Names (1)'!#REF!</xm:f>
           </x14:formula1>
-          <xm:sqref>B7:B8 B10 B17 B20:B23 B25:B29 B31:B32 B37 B40 B44 B48:B49 B51:B52 B54 B56:B57 B59:B62 B64:B69 B71:B75 B77:B81</xm:sqref>
+          <xm:sqref>B7:B8 B10 B17 B20:B23 B25:B29 B31:B32 B37 B40 B44 B48:B49 B51:B52 B54 B56:B57 B59:B62 B64:B69 B71:B75 B77:B82</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000005000000}">
           <x14:formula1>

</xml_diff>